<commit_message>
Fixed formatting issues with the following files
</commit_message>
<xml_diff>
--- a/Visualization Datasets/instiution count data.xlsx
+++ b/Visualization Datasets/instiution count data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Work\Python Projects\DS105-Data-Storage\Visualization Datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A45F4D4-D5A4-4151-A9CD-490BCBB8B4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -172,8 +178,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +242,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -282,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,9 +328,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,6 +380,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -523,14 +573,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="19" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>1996</v>
       </c>
@@ -586,7 +642,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -704,7 +760,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -763,7 +819,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -822,7 +878,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -881,7 +937,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -940,7 +996,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -999,7 +1055,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1176,7 +1232,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1235,7 +1291,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1294,7 +1350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1409,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1412,7 +1468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1471,7 +1527,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1530,7 +1586,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1589,7 +1645,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1648,7 +1704,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1707,7 +1763,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1766,7 +1822,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1825,7 +1881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1884,7 +1940,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1943,7 +1999,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2002,7 +2058,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2061,7 +2117,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2120,7 +2176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2179,7 +2235,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2238,7 +2294,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2297,7 +2353,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2356,7 +2412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -2415,7 +2471,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +2530,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2533,7 +2589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2592,7 +2648,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2651,7 +2707,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2766,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2769,7 +2825,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2828,7 +2884,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2887,7 +2943,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2946,7 +3002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -3005,7 +3061,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -3064,7 +3120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -3123,7 +3179,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -3182,7 +3238,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -3241,7 +3297,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -3300,7 +3356,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -3359,7 +3415,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -3418,7 +3474,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -3477,7 +3533,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -3536,7 +3592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>